<commit_message>
Fix bug in quad protocol
</commit_message>
<xml_diff>
--- a/Multicolor_particle_calibration.xlsx
+++ b/Multicolor_particle_calibration.xlsx
@@ -257,482 +257,482 @@
     </comment>
     <comment ref="B10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A1</t>
       </text>
     </comment>
     <comment ref="C10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A2</t>
       </text>
     </comment>
     <comment ref="D10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A3</t>
       </text>
     </comment>
     <comment ref="E10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A4</t>
       </text>
     </comment>
     <comment ref="F10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A5</t>
       </text>
     </comment>
     <comment ref="G10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A6</t>
       </text>
     </comment>
     <comment ref="H10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A7</t>
       </text>
     </comment>
     <comment ref="I10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A8</t>
       </text>
     </comment>
     <comment ref="J10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A9</t>
       </text>
     </comment>
     <comment ref="K10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A10</t>
       </text>
     </comment>
     <comment ref="L10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A11</t>
       </text>
     </comment>
     <comment ref="M10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_E12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_A12</t>
       </text>
     </comment>
     <comment ref="B11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B1</t>
       </text>
     </comment>
     <comment ref="C11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B2</t>
       </text>
     </comment>
     <comment ref="D11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B3</t>
       </text>
     </comment>
     <comment ref="E11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B4</t>
       </text>
     </comment>
     <comment ref="F11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B5</t>
       </text>
     </comment>
     <comment ref="G11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B6</t>
       </text>
     </comment>
     <comment ref="H11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B7</t>
       </text>
     </comment>
     <comment ref="I11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B8</t>
       </text>
     </comment>
     <comment ref="J11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B9</t>
       </text>
     </comment>
     <comment ref="K11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B10</t>
       </text>
     </comment>
     <comment ref="L11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B11</t>
       </text>
     </comment>
     <comment ref="M11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_F12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_B12</t>
       </text>
     </comment>
     <comment ref="B16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G1</t>
       </text>
     </comment>
     <comment ref="C16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G2</t>
       </text>
     </comment>
     <comment ref="D16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G3</t>
       </text>
     </comment>
     <comment ref="E16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G4</t>
       </text>
     </comment>
     <comment ref="F16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G5</t>
       </text>
     </comment>
     <comment ref="G16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G6</t>
       </text>
     </comment>
     <comment ref="H16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G7</t>
       </text>
     </comment>
     <comment ref="I16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G8</t>
       </text>
     </comment>
     <comment ref="J16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G9</t>
       </text>
     </comment>
     <comment ref="K16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G10</t>
       </text>
     </comment>
     <comment ref="L16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G11</t>
       </text>
     </comment>
     <comment ref="M16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_C12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_G12</t>
       </text>
     </comment>
     <comment ref="B17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H1</t>
       </text>
     </comment>
     <comment ref="C17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H2</t>
       </text>
     </comment>
     <comment ref="D17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H3</t>
       </text>
     </comment>
     <comment ref="E17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H4</t>
       </text>
     </comment>
     <comment ref="F17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H5</t>
       </text>
     </comment>
     <comment ref="G17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H6</t>
       </text>
     </comment>
     <comment ref="H17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H7</t>
       </text>
     </comment>
     <comment ref="I17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H8</t>
       </text>
     </comment>
     <comment ref="J17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H9</t>
       </text>
     </comment>
     <comment ref="K17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H10</t>
       </text>
     </comment>
     <comment ref="L17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H11</t>
       </text>
     </comment>
     <comment ref="M17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_D12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_H12</t>
       </text>
     </comment>
     <comment ref="B22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C1</t>
       </text>
     </comment>
     <comment ref="C22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C2</t>
       </text>
     </comment>
     <comment ref="D22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C3</t>
       </text>
     </comment>
     <comment ref="E22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C4</t>
       </text>
     </comment>
     <comment ref="F22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C5</t>
       </text>
     </comment>
     <comment ref="G22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C6</t>
       </text>
     </comment>
     <comment ref="H22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C7</t>
       </text>
     </comment>
     <comment ref="I22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C8</t>
       </text>
     </comment>
     <comment ref="J22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C9</t>
       </text>
     </comment>
     <comment ref="K22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C10</t>
       </text>
     </comment>
     <comment ref="L22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C11</t>
       </text>
     </comment>
     <comment ref="M22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_G12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_C12</t>
       </text>
     </comment>
     <comment ref="B23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D1</t>
       </text>
     </comment>
     <comment ref="C23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D2</t>
       </text>
     </comment>
     <comment ref="D23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D3</t>
       </text>
     </comment>
     <comment ref="E23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D4</t>
       </text>
     </comment>
     <comment ref="F23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D5</t>
       </text>
     </comment>
     <comment ref="G23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D6</t>
       </text>
     </comment>
     <comment ref="H23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D7</t>
       </text>
     </comment>
     <comment ref="I23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D8</t>
       </text>
     </comment>
     <comment ref="J23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D9</t>
       </text>
     </comment>
     <comment ref="K23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D10</t>
       </text>
     </comment>
     <comment ref="L23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D11</t>
       </text>
     </comment>
     <comment ref="M23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_H12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_D12</t>
       </text>
     </comment>
     <comment ref="B28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E1</t>
       </text>
     </comment>
     <comment ref="C28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E2</t>
       </text>
     </comment>
     <comment ref="D28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E3</t>
       </text>
     </comment>
     <comment ref="E28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E4</t>
       </text>
     </comment>
     <comment ref="F28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E5</t>
       </text>
     </comment>
     <comment ref="G28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E6</t>
       </text>
     </comment>
     <comment ref="H28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E7</t>
       </text>
     </comment>
     <comment ref="I28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E8</t>
       </text>
     </comment>
     <comment ref="J28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E9</t>
       </text>
     </comment>
     <comment ref="K28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E10</t>
       </text>
     </comment>
     <comment ref="L28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E11</t>
       </text>
     </comment>
     <comment ref="M28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_A12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_E12</t>
       </text>
     </comment>
     <comment ref="B29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F1</t>
       </text>
     </comment>
     <comment ref="C29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F2</t>
       </text>
     </comment>
     <comment ref="D29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F3</t>
       </text>
     </comment>
     <comment ref="E29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F4</t>
       </text>
     </comment>
     <comment ref="F29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F5</t>
       </text>
     </comment>
     <comment ref="G29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F6</t>
       </text>
     </comment>
     <comment ref="H29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F7</t>
       </text>
     </comment>
     <comment ref="I29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F8</t>
       </text>
     </comment>
     <comment ref="J29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F9</t>
       </text>
     </comment>
     <comment ref="K29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F10</t>
       </text>
     </comment>
     <comment ref="L29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F11</t>
       </text>
     </comment>
     <comment ref="M29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container5_B12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container3_F12</t>
       </text>
     </comment>
   </commentList>
@@ -1179,7 +1179,7 @@
     <row r="10">
       <c r="A10" s="10" t="inlineStr">
         <is>
-          <t>E</t>
+          <t>A</t>
         </is>
       </c>
       <c r="B10" s="11" t="n"/>
@@ -1198,7 +1198,7 @@
     <row r="11">
       <c r="A11" s="10" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>B</t>
         </is>
       </c>
       <c r="B11" s="11" t="n"/>
@@ -1293,7 +1293,7 @@
     <row r="16">
       <c r="A16" s="10" t="inlineStr">
         <is>
-          <t>C</t>
+          <t>G</t>
         </is>
       </c>
       <c r="B16" s="11" t="n"/>
@@ -1312,7 +1312,7 @@
     <row r="17">
       <c r="A17" s="10" t="inlineStr">
         <is>
-          <t>D</t>
+          <t>H</t>
         </is>
       </c>
       <c r="B17" s="11" t="n"/>
@@ -1407,7 +1407,7 @@
     <row r="22">
       <c r="A22" s="10" t="inlineStr">
         <is>
-          <t>G</t>
+          <t>C</t>
         </is>
       </c>
       <c r="B22" s="11" t="n"/>
@@ -1426,7 +1426,7 @@
     <row r="23">
       <c r="A23" s="10" t="inlineStr">
         <is>
-          <t>H</t>
+          <t>D</t>
         </is>
       </c>
       <c r="B23" s="11" t="n"/>
@@ -1521,7 +1521,7 @@
     <row r="28">
       <c r="A28" s="10" t="inlineStr">
         <is>
-          <t>A</t>
+          <t>E</t>
         </is>
       </c>
       <c r="B28" s="11" t="n"/>
@@ -1540,7 +1540,7 @@
     <row r="29">
       <c r="A29" s="10" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>F</t>
         </is>
       </c>
       <c r="B29" s="11" t="n"/>

</xml_diff>

<commit_message>
Added missing constraints, platereader emission bandwidth
</commit_message>
<xml_diff>
--- a/Multicolor_particle_calibration.xlsx
+++ b/Multicolor_particle_calibration.xlsx
@@ -257,482 +257,482 @@
     </comment>
     <comment ref="B10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A1</t>
       </text>
     </comment>
     <comment ref="C10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A2</t>
       </text>
     </comment>
     <comment ref="D10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A3</t>
       </text>
     </comment>
     <comment ref="E10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A4</t>
       </text>
     </comment>
     <comment ref="F10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A5</t>
       </text>
     </comment>
     <comment ref="G10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A6</t>
       </text>
     </comment>
     <comment ref="H10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A7</t>
       </text>
     </comment>
     <comment ref="I10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A8</t>
       </text>
     </comment>
     <comment ref="J10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A9</t>
       </text>
     </comment>
     <comment ref="K10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A10</t>
       </text>
     </comment>
     <comment ref="L10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A11</t>
       </text>
     </comment>
     <comment ref="M10" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_A12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_A12</t>
       </text>
     </comment>
     <comment ref="B11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B1</t>
       </text>
     </comment>
     <comment ref="C11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B2</t>
       </text>
     </comment>
     <comment ref="D11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B3</t>
       </text>
     </comment>
     <comment ref="E11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B4</t>
       </text>
     </comment>
     <comment ref="F11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B5</t>
       </text>
     </comment>
     <comment ref="G11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B6</t>
       </text>
     </comment>
     <comment ref="H11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B7</t>
       </text>
     </comment>
     <comment ref="I11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B8</t>
       </text>
     </comment>
     <comment ref="J11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B9</t>
       </text>
     </comment>
     <comment ref="K11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B10</t>
       </text>
     </comment>
     <comment ref="L11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B11</t>
       </text>
     </comment>
     <comment ref="M11" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_B12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_B12</t>
       </text>
     </comment>
     <comment ref="B16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C1</t>
       </text>
     </comment>
     <comment ref="C16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C2</t>
       </text>
     </comment>
     <comment ref="D16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C3</t>
       </text>
     </comment>
     <comment ref="E16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C4</t>
       </text>
     </comment>
     <comment ref="F16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C5</t>
       </text>
     </comment>
     <comment ref="G16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C6</t>
       </text>
     </comment>
     <comment ref="H16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C7</t>
       </text>
     </comment>
     <comment ref="I16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C8</t>
       </text>
     </comment>
     <comment ref="J16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C9</t>
       </text>
     </comment>
     <comment ref="K16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C10</t>
       </text>
     </comment>
     <comment ref="L16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C11</t>
       </text>
     </comment>
     <comment ref="M16" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_C12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_C12</t>
       </text>
     </comment>
     <comment ref="B17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D1</t>
       </text>
     </comment>
     <comment ref="C17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D2</t>
       </text>
     </comment>
     <comment ref="D17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D3</t>
       </text>
     </comment>
     <comment ref="E17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D4</t>
       </text>
     </comment>
     <comment ref="F17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D5</t>
       </text>
     </comment>
     <comment ref="G17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D6</t>
       </text>
     </comment>
     <comment ref="H17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D7</t>
       </text>
     </comment>
     <comment ref="I17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D8</t>
       </text>
     </comment>
     <comment ref="J17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D9</t>
       </text>
     </comment>
     <comment ref="K17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D10</t>
       </text>
     </comment>
     <comment ref="L17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D11</t>
       </text>
     </comment>
     <comment ref="M17" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_D12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_D12</t>
       </text>
     </comment>
     <comment ref="B22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E1</t>
       </text>
     </comment>
     <comment ref="C22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E2</t>
       </text>
     </comment>
     <comment ref="D22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E3</t>
       </text>
     </comment>
     <comment ref="E22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E4</t>
       </text>
     </comment>
     <comment ref="F22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E5</t>
       </text>
     </comment>
     <comment ref="G22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E6</t>
       </text>
     </comment>
     <comment ref="H22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E7</t>
       </text>
     </comment>
     <comment ref="I22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E8</t>
       </text>
     </comment>
     <comment ref="J22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E9</t>
       </text>
     </comment>
     <comment ref="K22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E10</t>
       </text>
     </comment>
     <comment ref="L22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E11</t>
       </text>
     </comment>
     <comment ref="M22" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_E12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_E12</t>
       </text>
     </comment>
     <comment ref="B23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F1</t>
       </text>
     </comment>
     <comment ref="C23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F2</t>
       </text>
     </comment>
     <comment ref="D23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F3</t>
       </text>
     </comment>
     <comment ref="E23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F4</t>
       </text>
     </comment>
     <comment ref="F23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F5</t>
       </text>
     </comment>
     <comment ref="G23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F6</t>
       </text>
     </comment>
     <comment ref="H23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F7</t>
       </text>
     </comment>
     <comment ref="I23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F8</t>
       </text>
     </comment>
     <comment ref="J23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F9</t>
       </text>
     </comment>
     <comment ref="K23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F10</t>
       </text>
     </comment>
     <comment ref="L23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F11</t>
       </text>
     </comment>
     <comment ref="M23" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_F12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_F12</t>
       </text>
     </comment>
     <comment ref="B28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G1</t>
       </text>
     </comment>
     <comment ref="C28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G2</t>
       </text>
     </comment>
     <comment ref="D28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G3</t>
       </text>
     </comment>
     <comment ref="E28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G4</t>
       </text>
     </comment>
     <comment ref="F28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G5</t>
       </text>
     </comment>
     <comment ref="G28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G6</t>
       </text>
     </comment>
     <comment ref="H28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G7</t>
       </text>
     </comment>
     <comment ref="I28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G8</t>
       </text>
     </comment>
     <comment ref="J28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G9</t>
       </text>
     </comment>
     <comment ref="K28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G10</t>
       </text>
     </comment>
     <comment ref="L28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G11</t>
       </text>
     </comment>
     <comment ref="M28" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_G12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_G12</t>
       </text>
     </comment>
     <comment ref="B29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H1</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H1</t>
       </text>
     </comment>
     <comment ref="C29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H2</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H2</t>
       </text>
     </comment>
     <comment ref="D29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H3</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H3</t>
       </text>
     </comment>
     <comment ref="E29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H4</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H4</t>
       </text>
     </comment>
     <comment ref="F29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H5</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H5</t>
       </text>
     </comment>
     <comment ref="G29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H6</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H6</t>
       </text>
     </comment>
     <comment ref="H29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H7</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H7</t>
       </text>
     </comment>
     <comment ref="I29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H8</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H8</t>
       </text>
     </comment>
     <comment ref="J29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H9</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H9</t>
       </text>
     </comment>
     <comment ref="K29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H10</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H10</t>
       </text>
     </comment>
     <comment ref="L29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H11</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H11</t>
       </text>
     </comment>
     <comment ref="M29" authorId="0" shapeId="0">
       <text>
-        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container2_H12</t>
+        <t>https://igem.org/Engineering/protocols/Multicolor_particle_calibration/Container4_H12</t>
       </text>
     </comment>
   </commentList>

</xml_diff>